<commit_message>
WareMap v 1.0 finalized
</commit_message>
<xml_diff>
--- a/src/main/resources/temp/ordercharger.xlsx
+++ b/src/main/resources/temp/ordercharger.xlsx
@@ -30,9 +30,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
   <si>
     <t>minhoca suja de barro</t>
+  </si>
+  <si>
+    <t>presunto oval</t>
+  </si>
+  <si>
+    <t>bacon fracionado</t>
+  </si>
+  <si>
+    <t>bacon manta</t>
+  </si>
+  <si>
+    <t>cuzcuz de flocao</t>
+  </si>
+  <si>
+    <t xml:space="preserve">teste </t>
   </si>
 </sst>
 </file>
@@ -381,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -469,6 +484,61 @@
         <v>50</v>
       </c>
     </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1">
+        <v>4021</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1">
+        <v>5023</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="1">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1">
+        <v>5009</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="1">
+        <v>4016</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1">
+        <v>8005</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="1">
+        <v>120</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
Versao com correcao de alguns erros. estavel
</commit_message>
<xml_diff>
--- a/src/main/resources/temp/ordercharger.xlsx
+++ b/src/main/resources/temp/ordercharger.xlsx
@@ -4,50 +4,57 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" iterateDelta="1E-4"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
-  <si>
-    <t>minhoca suja de barro</t>
-  </si>
-  <si>
-    <t>presunto oval</t>
-  </si>
-  <si>
-    <t>bacon fracionado</t>
-  </si>
-  <si>
-    <t>bacon manta</t>
-  </si>
-  <si>
-    <t>cuzcuz de flocao</t>
-  </si>
-  <si>
-    <t xml:space="preserve">teste </t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>COXA C/ SOBRECOXA FRANGO CONGELADO CX. 20KG</t>
+  </si>
+  <si>
+    <t>FILE DE PEITO FRANGO CONGELADO CX. 20KG</t>
+  </si>
+  <si>
+    <t>FILE DE PEITO FRANGO CONGELADO BANDEJA</t>
+  </si>
+  <si>
+    <t>DORSO FRANGO CONGELADO CX. 17KG</t>
+  </si>
+  <si>
+    <t>FRANGO CONGELADO CX. 20KG</t>
+  </si>
+  <si>
+    <t>FILE DE PEITO FRANGO CONG. INTERFOLHADO CX. 20KG</t>
+  </si>
+  <si>
+    <t>SOBRECOXA FRANGO RESFRIADA CX. 20KG</t>
+  </si>
+  <si>
+    <t>PEITO FRANGO CONGELADO INDIVIDUAL CX. 20 KG</t>
+  </si>
+  <si>
+    <t>FILE DE SASSAMI FRANGO CONGELADO INTERFOLHADO CX. 20KG</t>
+  </si>
+  <si>
+    <t>CMS CONGELADO CX 20KG</t>
+  </si>
+  <si>
+    <t>BACON DE PALETA</t>
+  </si>
+  <si>
+    <t>picanha</t>
   </si>
 </sst>
 </file>
@@ -91,9 +98,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,139 +412,139 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="2" max="2" width="57.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="1">
+      <c r="A1" s="2">
         <v>11007</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1">
-        <v>80</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="1">
+      <c r="A2" s="2">
+        <v>11015</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="2">
+        <v>11016</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="2">
+        <v>11023</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="2">
         <v>11046</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1">
-        <v>11096</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1">
-        <v>11015</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="1">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1">
-        <v>11092</v>
-      </c>
       <c r="B5" s="1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1">
-        <v>50</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="1">
-        <v>11023</v>
+      <c r="A6" s="2">
+        <v>11068</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C6" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="2">
+        <v>11072</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="2">
+        <v>11076</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="2">
+        <v>11084</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="2">
+        <v>11085</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="1">
-        <v>11076</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="1">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="1">
-        <v>4021</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="1">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="1">
+    <row r="11" spans="1:3">
+      <c r="A11" s="2">
         <v>5023</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="1">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="1">
-        <v>5009</v>
-      </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="1">
         <v>3</v>
       </c>
-      <c r="C10" s="1">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="1">
-        <v>4016</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="1">
-        <v>32</v>
-      </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="1">
-        <v>8005</v>
+      <c r="A12" s="2">
+        <v>2003</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C12" s="1">
-        <v>120</v>
+        <v>800</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correção de erro ainda nao pronto!
</commit_message>
<xml_diff>
--- a/src/main/resources/temp/ordercharger.xlsx
+++ b/src/main/resources/temp/ordercharger.xlsx
@@ -19,42 +19,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>COXA C/ SOBRECOXA FRANGO CONGELADO CX. 20KG</t>
-  </si>
-  <si>
-    <t>FILE DE PEITO FRANGO CONGELADO CX. 20KG</t>
-  </si>
-  <si>
-    <t>FILE DE PEITO FRANGO CONGELADO BANDEJA</t>
-  </si>
-  <si>
-    <t>DORSO FRANGO CONGELADO CX. 17KG</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>FRANGO CONGELADO CX. 20KG</t>
-  </si>
-  <si>
-    <t>FILE DE PEITO FRANGO CONG. INTERFOLHADO CX. 20KG</t>
-  </si>
-  <si>
-    <t>SOBRECOXA FRANGO RESFRIADA CX. 20KG</t>
-  </si>
-  <si>
-    <t>PEITO FRANGO CONGELADO INDIVIDUAL CX. 20 KG</t>
-  </si>
-  <si>
-    <t>FILE DE SASSAMI FRANGO CONGELADO INTERFOLHADO CX. 20KG</t>
-  </si>
-  <si>
-    <t>CMS CONGELADO CX 20KG</t>
-  </si>
-  <si>
-    <t>BACON DE PALETA</t>
-  </si>
-  <si>
-    <t>picanha</t>
   </si>
 </sst>
 </file>
@@ -404,10 +371,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -416,136 +383,80 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="2">
-        <v>11007</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1">
-        <v>46</v>
-      </c>
+      <c r="A1" s="2"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="2">
-        <v>11015</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1">
-        <v>32</v>
-      </c>
+      <c r="A2" s="2"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="2">
-        <v>11016</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
+      <c r="A3" s="2"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="2">
-        <v>11023</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1">
-        <v>12</v>
-      </c>
+      <c r="A4" s="2"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2">
         <v>11046</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C5" s="1">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="2">
-        <v>11068</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1">
-        <v>32</v>
-      </c>
+      <c r="A6" s="2"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="2">
-        <v>11072</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1</v>
-      </c>
+      <c r="A7" s="2"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="2">
-        <v>11076</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="1">
-        <v>3</v>
-      </c>
+      <c r="A8" s="2"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="2">
-        <v>11084</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="1">
-        <v>5</v>
-      </c>
+      <c r="A9" s="2"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="2">
-        <v>11085</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="1">
-        <v>20</v>
-      </c>
+      <c r="A10" s="2"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="2">
-        <v>5023</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="1">
-        <v>30</v>
-      </c>
+      <c r="A11" s="2"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="2">
-        <v>2003</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="1">
-        <v>800</v>
-      </c>
+      <c r="A12" s="2"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="2"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="2"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Versao estavel (NAo foi detectados bug's)
</commit_message>
<xml_diff>
--- a/src/main/resources/temp/ordercharger.xlsx
+++ b/src/main/resources/temp/ordercharger.xlsx
@@ -19,9 +19,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+  <si>
+    <t>COXA C/ SOBRECOXA FRANGO CONGELADO CX. 20KG</t>
+  </si>
+  <si>
+    <t>FILE DE PEITO FRANGO CONGELADO CX. 20KG</t>
+  </si>
+  <si>
+    <t>FILE DE PEITO FRANGO CONGELADO BANDEJA</t>
+  </si>
+  <si>
+    <t>DORSO FRANGO CONGELADO CX. 17KG</t>
+  </si>
   <si>
     <t>FRANGO CONGELADO CX. 20KG</t>
+  </si>
+  <si>
+    <t>FILE DE PEITO FRANGO CONG. INTERFOLHADO CX. 20KG</t>
+  </si>
+  <si>
+    <t>SOBRECOXA FRANGO RESFRIADA CX. 20KG</t>
+  </si>
+  <si>
+    <t>PEITO FRANGO CONGELADO INDIVIDUAL CX. 20 KG</t>
+  </si>
+  <si>
+    <t>FILE DE SASSAMI FRANGO CONGELADO INTERFOLHADO CX. 20KG</t>
+  </si>
+  <si>
+    <t>CMS CONGELADO CX 20KG</t>
+  </si>
+  <si>
+    <t>BACON DE PALETA</t>
+  </si>
+  <si>
+    <t>picanha</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -374,7 +410,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -383,80 +419,158 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="2"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
+      <c r="A1" s="2">
+        <v>11007</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1">
+        <v>46</v>
+      </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="2"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
+      <c r="A2" s="2">
+        <v>11015</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>32</v>
+      </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+      <c r="A3" s="2">
+        <v>11016</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="2"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
+      <c r="A4" s="2">
+        <v>11023</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>12</v>
+      </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2">
         <v>11046</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="2"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
+      <c r="A6" s="2">
+        <v>11068</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1">
+        <v>32</v>
+      </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="2"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="A7" s="2">
+        <v>11072</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="2"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
+      <c r="A8" s="2">
+        <v>11076</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="2"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
+      <c r="A9" s="2">
+        <v>11084</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="2"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
+      <c r="A10" s="2">
+        <v>11085</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1">
+        <v>20</v>
+      </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="2"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
+      <c r="A11" s="2">
+        <v>5023</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="1">
+        <v>30</v>
+      </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="2"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
+      <c r="A12" s="2">
+        <v>2003</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="1">
+        <v>800</v>
+      </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="2"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
+      <c r="A13" s="2">
+        <v>5015</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="1">
+        <v>56</v>
+      </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="2"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+      <c r="A14" s="2">
+        <v>11074</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="1">
+        <v>400</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
criando a tela para informar quantidade individual frango.
</commit_message>
<xml_diff>
--- a/src/main/resources/temp/ordercharger.xlsx
+++ b/src/main/resources/temp/ordercharger.xlsx
@@ -19,40 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>COXA C/ SOBRECOXA FRANGO CONGELADO CX. 20KG</t>
-  </si>
-  <si>
-    <t>FILE DE PEITO FRANGO CONGELADO CX. 20KG</t>
-  </si>
-  <si>
-    <t>FILE DE PEITO FRANGO CONGELADO BANDEJA</t>
-  </si>
-  <si>
-    <t>DORSO FRANGO CONGELADO CX. 17KG</t>
-  </si>
-  <si>
-    <t>FRANGO CONGELADO CX. 20KG</t>
-  </si>
-  <si>
-    <t>FILE DE PEITO FRANGO CONG. INTERFOLHADO CX. 20KG</t>
-  </si>
-  <si>
-    <t>SOBRECOXA FRANGO RESFRIADA CX. 20KG</t>
-  </si>
-  <si>
-    <t>PEITO FRANGO CONGELADO INDIVIDUAL CX. 20 KG</t>
-  </si>
-  <si>
-    <t>FILE DE SASSAMI FRANGO CONGELADO INTERFOLHADO CX. 20KG</t>
-  </si>
-  <si>
-    <t>CMS CONGELADO CX 20KG</t>
-  </si>
-  <si>
-    <t>BACON DE PALETA</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>picanha</t>
   </si>
@@ -404,10 +371,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -417,135 +384,64 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2">
-        <v>11007</v>
+        <v>11046</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="2">
-        <v>11015</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="2">
-        <v>11016</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="2">
-        <v>11023</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="2">
-        <v>11046</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="2">
-        <v>11068</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="2">
-        <v>11072</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="2">
-        <v>11076</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="2">
-        <v>11084</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="2">
-        <v>11085</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="2">
-        <v>5023</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="2">
-        <v>2003</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="1">
         <v>800</v>
       </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="2"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="2"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="2"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="2"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="2"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="2"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="2"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>